<commit_message>
Add excelFormatCopy option and fix apex class and apex page output for n/a
</commit_message>
<xml_diff>
--- a/configs/ja/template_ja.xlsx
+++ b/configs/ja/template_ja.xlsx
@@ -798,38 +798,38 @@
         <v>1</v>
       </c>
       <c r="E4" s="18"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
-      <c r="W4" s="2"/>
-      <c r="X4" s="2"/>
-      <c r="Y4" s="2"/>
-      <c r="Z4" s="2"/>
-      <c r="AA4" s="2"/>
-      <c r="AB4" s="2"/>
-      <c r="AC4" s="2"/>
-      <c r="AD4" s="2"/>
-      <c r="AE4" s="2"/>
-      <c r="AF4" s="2"/>
-      <c r="AG4" s="2"/>
-      <c r="AH4" s="2"/>
-      <c r="AI4" s="2"/>
-      <c r="AJ4" s="2"/>
-      <c r="AK4" s="2"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="9"/>
+      <c r="W4" s="9"/>
+      <c r="X4" s="9"/>
+      <c r="Y4" s="9"/>
+      <c r="Z4" s="9"/>
+      <c r="AA4" s="9"/>
+      <c r="AB4" s="9"/>
+      <c r="AC4" s="9"/>
+      <c r="AD4" s="9"/>
+      <c r="AE4" s="9"/>
+      <c r="AF4" s="9"/>
+      <c r="AG4" s="9"/>
+      <c r="AH4" s="9"/>
+      <c r="AI4" s="9"/>
+      <c r="AJ4" s="9"/>
+      <c r="AK4" s="9"/>
     </row>
     <row r="5" spans="1:37" ht="17.399999999999999" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>

</xml_diff>

<commit_message>
Changed Excel library and added output functionality for Custom Metadata Type Access, Custom Setting Access, and Login Hours
</commit_message>
<xml_diff>
--- a/configs/ja/template_ja.xlsx
+++ b/configs/ja/template_ja.xlsx
@@ -7,10 +7,10 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8916"/>
   </bookViews>
   <sheets>
-    <sheet name="Output results" sheetId="1" r:id="rId1"/>
+    <sheet name="output results" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Output results'!$A$6:$AK$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'output results'!$A$6:$AK$6</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -798,38 +798,38 @@
         <v>1</v>
       </c>
       <c r="E4" s="18"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="9"/>
-      <c r="S4" s="9"/>
-      <c r="T4" s="9"/>
-      <c r="U4" s="9"/>
-      <c r="V4" s="9"/>
-      <c r="W4" s="9"/>
-      <c r="X4" s="9"/>
-      <c r="Y4" s="9"/>
-      <c r="Z4" s="9"/>
-      <c r="AA4" s="9"/>
-      <c r="AB4" s="9"/>
-      <c r="AC4" s="9"/>
-      <c r="AD4" s="9"/>
-      <c r="AE4" s="9"/>
-      <c r="AF4" s="9"/>
-      <c r="AG4" s="9"/>
-      <c r="AH4" s="9"/>
-      <c r="AI4" s="9"/>
-      <c r="AJ4" s="9"/>
-      <c r="AK4" s="9"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="2"/>
+      <c r="AF4" s="2"/>
+      <c r="AG4" s="2"/>
+      <c r="AH4" s="2"/>
+      <c r="AI4" s="2"/>
+      <c r="AJ4" s="2"/>
+      <c r="AK4" s="2"/>
     </row>
     <row r="5" spans="1:37" ht="17.399999999999999" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>

</xml_diff>